<commit_message>
Agregando textos al lexicon
</commit_message>
<xml_diff>
--- a/demo_lexicon/Lexicon.xlsx
+++ b/demo_lexicon/Lexicon.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\unmsm\Thesis_project_QuispeCabello_Sanchez_Wong\demo_lexicon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB4CE42-31AC-4206-A4CF-9B4E5E66670B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F26554E-E7F2-455C-82D0-D3D6A5DAA89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{9B249666-9A8A-4383-8168-2FD58BE5AA28}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2076" uniqueCount="1014">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="1114">
   <si>
     <t>Text</t>
   </si>
@@ -3081,6 +3081,306 @@
   </si>
   <si>
     <t>espera</t>
+  </si>
+  <si>
+    <t>mejor opcion</t>
+  </si>
+  <si>
+    <t>lider</t>
+  </si>
+  <si>
+    <t>no servicio</t>
+  </si>
+  <si>
+    <t>feliz</t>
+  </si>
+  <si>
+    <t>agradable</t>
+  </si>
+  <si>
+    <t>gran servicio</t>
+  </si>
+  <si>
+    <t>acuerdo</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>guau</t>
+  </si>
+  <si>
+    <t>promedio</t>
+  </si>
+  <si>
+    <t>inhumano</t>
+  </si>
+  <si>
+    <t>si poder poner</t>
+  </si>
+  <si>
+    <t>excusa</t>
+  </si>
+  <si>
+    <t>beneficio</t>
+  </si>
+  <si>
+    <t>ineficiente</t>
+  </si>
+  <si>
+    <t>nefasto</t>
+  </si>
+  <si>
+    <t>ni contestan</t>
+  </si>
+  <si>
+    <t>poco profesional</t>
+  </si>
+  <si>
+    <t>mediocre</t>
+  </si>
+  <si>
+    <t>nulo</t>
+  </si>
+  <si>
+    <t>tarde</t>
+  </si>
+  <si>
+    <t>cero apoyo</t>
+  </si>
+  <si>
+    <t>sin apoyo</t>
+  </si>
+  <si>
+    <t>casi hora</t>
+  </si>
+  <si>
+    <t>mala gana</t>
+  </si>
+  <si>
+    <t>no sincero</t>
+  </si>
+  <si>
+    <t>alargar</t>
+  </si>
+  <si>
+    <t>no mostrar</t>
+  </si>
+  <si>
+    <t>limitar</t>
+  </si>
+  <si>
+    <t>dificil</t>
+  </si>
+  <si>
+    <t>nadie contestar</t>
+  </si>
+  <si>
+    <t>cansir</t>
+  </si>
+  <si>
+    <t>perdi</t>
+  </si>
+  <si>
+    <t>cambiense</t>
+  </si>
+  <si>
+    <t>tirar</t>
+  </si>
+  <si>
+    <t>tirar plata</t>
+  </si>
+  <si>
+    <t>maltrato</t>
+  </si>
+  <si>
+    <t>mediocr</t>
+  </si>
+  <si>
+    <t>no funcionar</t>
+  </si>
+  <si>
+    <t>frio</t>
+  </si>
+  <si>
+    <t>tratar amabilidad</t>
+  </si>
+  <si>
+    <t>capacitar</t>
+  </si>
+  <si>
+    <t>no venir</t>
+  </si>
+  <si>
+    <t>tratar</t>
+  </si>
+  <si>
+    <t>no reconocer</t>
+  </si>
+  <si>
+    <t>servicial</t>
+  </si>
+  <si>
+    <t>organizado</t>
+  </si>
+  <si>
+    <t>concis</t>
+  </si>
+  <si>
+    <t>detallado</t>
+  </si>
+  <si>
+    <t>trabar</t>
+  </si>
+  <si>
+    <t>no agrado</t>
+  </si>
+  <si>
+    <t>no señal</t>
+  </si>
+  <si>
+    <t>no poder creer</t>
+  </si>
+  <si>
+    <t>decir gran empresa</t>
+  </si>
+  <si>
+    <t>no tener personal calificado</t>
+  </si>
+  <si>
+    <t>amablemente</t>
+  </si>
+  <si>
+    <t>exelente</t>
+  </si>
+  <si>
+    <t>cualquiera cosa</t>
+  </si>
+  <si>
+    <t>preocupado</t>
+  </si>
+  <si>
+    <t>medio hora</t>
+  </si>
+  <si>
+    <t>no primero vez</t>
+  </si>
+  <si>
+    <t>cualquiera</t>
+  </si>
+  <si>
+    <t>cualquier</t>
+  </si>
+  <si>
+    <t>bonito</t>
+  </si>
+  <si>
+    <t>resguardado</t>
+  </si>
+  <si>
+    <t>poco tiempo espera</t>
+  </si>
+  <si>
+    <t>correctamente</t>
+  </si>
+  <si>
+    <t>facil perder</t>
+  </si>
+  <si>
+    <t>limpieza</t>
+  </si>
+  <si>
+    <t>agil</t>
+  </si>
+  <si>
+    <t>broma</t>
+  </si>
+  <si>
+    <t>sensibilidad</t>
+  </si>
+  <si>
+    <t>querer pagar</t>
+  </si>
+  <si>
+    <t>deber brindar</t>
+  </si>
+  <si>
+    <t>llamar varios vez</t>
+  </si>
+  <si>
+    <t>faltar buen</t>
+  </si>
+  <si>
+    <t>faltar buen atencion</t>
+  </si>
+  <si>
+    <t>faltar buen atencion personalizado</t>
+  </si>
+  <si>
+    <t>no orientacion</t>
+  </si>
+  <si>
+    <t>no necesario</t>
+  </si>
+  <si>
+    <t>tiempo perdido</t>
+  </si>
+  <si>
+    <t>deber resolver</t>
+  </si>
+  <si>
+    <t>faltar veracidad</t>
+  </si>
+  <si>
+    <t>felizmente poder solucionar</t>
+  </si>
+  <si>
+    <t>total desorganizacion</t>
+  </si>
+  <si>
+    <t>no organización</t>
+  </si>
+  <si>
+    <t>porfavor</t>
+  </si>
+  <si>
+    <t>papeleo</t>
+  </si>
+  <si>
+    <t>grato</t>
+  </si>
+  <si>
+    <t>correcto</t>
+  </si>
+  <si>
+    <t>trato comunicar</t>
+  </si>
+  <si>
+    <t>trato llamar</t>
+  </si>
+  <si>
+    <t>trato contactar</t>
+  </si>
+  <si>
+    <t>no suficiente</t>
+  </si>
+  <si>
+    <t>tratar comunicar</t>
+  </si>
+  <si>
+    <t>tratar llamar</t>
+  </si>
+  <si>
+    <t>tratar contactar</t>
+  </si>
+  <si>
+    <t>perseverancia</t>
+  </si>
+  <si>
+    <t>esperar mucho</t>
+  </si>
+  <si>
+    <t>esperar demasiado</t>
   </si>
 </sst>
 </file>
@@ -11298,16 +11598,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F5993EC-C272-4BB3-8AF9-D99E2F29219A}">
-  <dimension ref="A1:K425"/>
+  <dimension ref="A1:K529"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
     <col min="3" max="3" width="25.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16103,6 +16403,1150 @@
         <v>0</v>
       </c>
       <c r="C425">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A426" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B426">
+        <v>1</v>
+      </c>
+      <c r="C426">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A427" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B427">
+        <v>1</v>
+      </c>
+      <c r="C427">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B428">
+        <v>0</v>
+      </c>
+      <c r="C428">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>575</v>
+      </c>
+      <c r="B429">
+        <v>0</v>
+      </c>
+      <c r="C429">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A430" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B430">
+        <v>1</v>
+      </c>
+      <c r="C430">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A431" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B431">
+        <v>1</v>
+      </c>
+      <c r="C431">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A432" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B432">
+        <v>1</v>
+      </c>
+      <c r="C432">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A433" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B433">
+        <v>1</v>
+      </c>
+      <c r="C433">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A434" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B434">
+        <v>0</v>
+      </c>
+      <c r="C434">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A435" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B435">
+        <v>1</v>
+      </c>
+      <c r="C435">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A436" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B436">
+        <v>0</v>
+      </c>
+      <c r="C436">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A437" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B437">
+        <v>0</v>
+      </c>
+      <c r="C437">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A438" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B438">
+        <v>0</v>
+      </c>
+      <c r="C438">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A439" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B439">
+        <v>0</v>
+      </c>
+      <c r="C439">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A440" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B440">
+        <v>1</v>
+      </c>
+      <c r="C440">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A441" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B441">
+        <v>0</v>
+      </c>
+      <c r="C441">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A442" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B442">
+        <v>0</v>
+      </c>
+      <c r="C442">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A443" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B443">
+        <v>0</v>
+      </c>
+      <c r="C443">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A444" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B444">
+        <v>0</v>
+      </c>
+      <c r="C444">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A445" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B445">
+        <v>0</v>
+      </c>
+      <c r="C445">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A446" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B446">
+        <v>0</v>
+      </c>
+      <c r="C446">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A447" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B447">
+        <v>0</v>
+      </c>
+      <c r="C447">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A448" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B448">
+        <v>0</v>
+      </c>
+      <c r="C448">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A449" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B449">
+        <v>0</v>
+      </c>
+      <c r="C449">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A450" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B450">
+        <v>0</v>
+      </c>
+      <c r="C450">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A451" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B451">
+        <v>0</v>
+      </c>
+      <c r="C451">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A452" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B452">
+        <v>0</v>
+      </c>
+      <c r="C452">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A453" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B453">
+        <v>0</v>
+      </c>
+      <c r="C453">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A454" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B454">
+        <v>0</v>
+      </c>
+      <c r="C454">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A455" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B455">
+        <v>0</v>
+      </c>
+      <c r="C455">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A456" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B456">
+        <v>0</v>
+      </c>
+      <c r="C456">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A457" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B457">
+        <v>0</v>
+      </c>
+      <c r="C457">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A458" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B458">
+        <v>0</v>
+      </c>
+      <c r="C458">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A459" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B459">
+        <v>0</v>
+      </c>
+      <c r="C459">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A460" t="s">
+        <v>895</v>
+      </c>
+      <c r="B460">
+        <v>0</v>
+      </c>
+      <c r="C460">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A461" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B461">
+        <v>0</v>
+      </c>
+      <c r="C461">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A462" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B462">
+        <v>0</v>
+      </c>
+      <c r="C462">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A463" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B463">
+        <v>0</v>
+      </c>
+      <c r="C463">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A464" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B464">
+        <v>0</v>
+      </c>
+      <c r="C464">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A465" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B465">
+        <v>0</v>
+      </c>
+      <c r="C465">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A466" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B466">
+        <v>0</v>
+      </c>
+      <c r="C466">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A467" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B467">
+        <v>0</v>
+      </c>
+      <c r="C467">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A468" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B468">
+        <v>0</v>
+      </c>
+      <c r="C468">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A469" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B469">
+        <v>0</v>
+      </c>
+      <c r="C469">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A470" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B470">
+        <v>0</v>
+      </c>
+      <c r="C470">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A471" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B471">
+        <v>0</v>
+      </c>
+      <c r="C471">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A472" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B472">
+        <v>0</v>
+      </c>
+      <c r="C472">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A473" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B473">
+        <v>1</v>
+      </c>
+      <c r="C473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A474" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B474">
+        <v>1</v>
+      </c>
+      <c r="C474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A475" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B475">
+        <v>1</v>
+      </c>
+      <c r="C475">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A476" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B476">
+        <v>1</v>
+      </c>
+      <c r="C476">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="477" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A477" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B477">
+        <v>0</v>
+      </c>
+      <c r="C477">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="478" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A478" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B478">
+        <v>0</v>
+      </c>
+      <c r="C478">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="479" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A479" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B479">
+        <v>0</v>
+      </c>
+      <c r="C479">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="480" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A480" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B480">
+        <v>0</v>
+      </c>
+      <c r="C480">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A481" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B481">
+        <v>0</v>
+      </c>
+      <c r="C481">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A482" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B482">
+        <v>0</v>
+      </c>
+      <c r="C482">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A483" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B483">
+        <v>1</v>
+      </c>
+      <c r="C483">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A484" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B484">
+        <v>1</v>
+      </c>
+      <c r="C484">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A485" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B485">
+        <v>0</v>
+      </c>
+      <c r="C485">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A486" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B486">
+        <v>0</v>
+      </c>
+      <c r="C486">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A487" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B487">
+        <v>0</v>
+      </c>
+      <c r="C487">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A488" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B488">
+        <v>0</v>
+      </c>
+      <c r="C488">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A489" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B489">
+        <v>0</v>
+      </c>
+      <c r="C489">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A490" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B490">
+        <v>0</v>
+      </c>
+      <c r="C490">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A491" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B491">
+        <v>1</v>
+      </c>
+      <c r="C491">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A492" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B492">
+        <v>1</v>
+      </c>
+      <c r="C492">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A493" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B493">
+        <v>1</v>
+      </c>
+      <c r="C493">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A494" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B494">
+        <v>1</v>
+      </c>
+      <c r="C494">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A495" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B495">
+        <v>0</v>
+      </c>
+      <c r="C495">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A496" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B496">
+        <v>1</v>
+      </c>
+      <c r="C496">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A497" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B497">
+        <v>1</v>
+      </c>
+      <c r="C497">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A498" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B498">
+        <v>0</v>
+      </c>
+      <c r="C498">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A499" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B499">
+        <v>1</v>
+      </c>
+      <c r="C499">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A500" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B500">
+        <v>0</v>
+      </c>
+      <c r="C500">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A501" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B501">
+        <v>0</v>
+      </c>
+      <c r="C501">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A502" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B502">
+        <v>0</v>
+      </c>
+      <c r="C502">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A503" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B503">
+        <v>0</v>
+      </c>
+      <c r="C503">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A504" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B504">
+        <v>0</v>
+      </c>
+      <c r="C504">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A505" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B505">
+        <v>0</v>
+      </c>
+      <c r="C505">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A506" t="s">
+        <v>304</v>
+      </c>
+      <c r="B506">
+        <v>0</v>
+      </c>
+      <c r="C506">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A507" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B507">
+        <v>0</v>
+      </c>
+      <c r="C507">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A508" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B508">
+        <v>0</v>
+      </c>
+      <c r="C508">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A509" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B509">
+        <v>0</v>
+      </c>
+      <c r="C509">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A510" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B510">
+        <v>0</v>
+      </c>
+      <c r="C510">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A511" t="s">
+        <v>615</v>
+      </c>
+      <c r="B511">
+        <v>1</v>
+      </c>
+      <c r="C511">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A512" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B512">
+        <v>0</v>
+      </c>
+      <c r="C512">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A513" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B513">
+        <v>1</v>
+      </c>
+      <c r="C513">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A514" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B514">
+        <v>0</v>
+      </c>
+      <c r="C514">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A515" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B515">
+        <v>0</v>
+      </c>
+      <c r="C515">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A516" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B516">
+        <v>0</v>
+      </c>
+      <c r="C516">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A517" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B517">
+        <v>0</v>
+      </c>
+      <c r="C517">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A518" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B518">
+        <v>1</v>
+      </c>
+      <c r="C518">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A519" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B519">
+        <v>1</v>
+      </c>
+      <c r="C519">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A520" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B520">
+        <v>0</v>
+      </c>
+      <c r="C520">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A521" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B521">
+        <v>0</v>
+      </c>
+      <c r="C521">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A522" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B522">
+        <v>0</v>
+      </c>
+      <c r="C522">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A523" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B523">
+        <v>0</v>
+      </c>
+      <c r="C523">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A524" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B524">
+        <v>0</v>
+      </c>
+      <c r="C524">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A525" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B525">
+        <v>0</v>
+      </c>
+      <c r="C525">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A526" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B526">
+        <v>0</v>
+      </c>
+      <c r="C526">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A527" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B527">
+        <v>0</v>
+      </c>
+      <c r="C527">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A528" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B528">
+        <v>0</v>
+      </c>
+      <c r="C528">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="529" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A529" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B529">
+        <v>0</v>
+      </c>
+      <c r="C529">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prueba lexicon new dataset
</commit_message>
<xml_diff>
--- a/demo_lexicon/Lexicon.xlsx
+++ b/demo_lexicon/Lexicon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\unmsm\Thesis_project_QuispeCabello_Sanchez_Wong\demo_lexicon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F26554E-E7F2-455C-82D0-D3D6A5DAA89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C776BA71-DC3A-42A5-A26F-31029DC6D49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{9B249666-9A8A-4383-8168-2FD58BE5AA28}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="lexicon_master" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">lexiconv2_lematizado!$B$1:$C$325</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">lexiconv2_lematizado!$A$1:$K$529</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -11601,7 +11601,7 @@
   <dimension ref="A1:K529"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15114,7 +15114,7 @@
         <v>0</v>
       </c>
       <c r="C310">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.3">
@@ -17551,6 +17551,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K529" xr:uid="{1F5993EC-C272-4BB3-8AF9-D99E2F29219A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K477">
     <sortCondition ref="A1:A477"/>
   </sortState>

</xml_diff>